<commit_message>
canceled Settle secured OD action verify
</commit_message>
<xml_diff>
--- a/Lending/Feature - List Services UIUX 04.01.2019 -Plan mapping code OCB.xlsx
+++ b/Lending/Feature - List Services UIUX 04.01.2019 -Plan mapping code OCB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces_2018\DemoSAP_UI5_Git\SAPUI_DEMO\Lending\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AE2D13-B183-4C5D-85C9-842967AEF5AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046067AB-4A2B-4307-A9F3-5BC5010892B4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="149">
   <si>
     <t>Module</t>
   </si>
@@ -457,9 +457,6 @@
   </si>
   <si>
     <t>UPL</t>
-  </si>
-  <si>
-    <t>WIP</t>
   </si>
   <si>
     <t>Open</t>
@@ -587,6 +584,12 @@
   </si>
   <si>
     <t xml:space="preserve">GetAccountDetailsByID  Service </t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>WIP</t>
   </si>
 </sst>
 </file>
@@ -2240,26 +2243,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-4437-44F0-AB86-16DD75D97B11}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -2316,21 +2299,13 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
+            <c:multiLvlStrRef>
               <c:f>Sheet1!$N$3:$N$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$O$3:$O$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -3334,7 +3309,7 @@
   <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L95" sqref="L95"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3394,7 +3369,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -3471,7 +3446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="114" t="s">
         <v>96</v>
       </c>
@@ -3628,7 +3603,7 @@
       <c r="L8" s="79"/>
       <c r="M8" s="79"/>
     </row>
-    <row r="9" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="112" t="s">
         <v>6</v>
       </c>
@@ -3687,7 +3662,7 @@
       <c r="L10" s="79"/>
       <c r="M10" s="79"/>
     </row>
-    <row r="11" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="112" t="s">
         <v>6</v>
       </c>
@@ -3750,7 +3725,7 @@
         <v>43479</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="112" t="s">
         <v>6</v>
       </c>
@@ -3995,7 +3970,7 @@
       <c r="L21" s="79"/>
       <c r="M21" s="79"/>
     </row>
-    <row r="22" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
         <v>6</v>
       </c>
@@ -4018,7 +3993,7 @@
       </c>
       <c r="I22" s="42"/>
       <c r="J22" s="59" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="K22" s="41" t="s">
         <v>107</v>
@@ -4108,7 +4083,7 @@
       <c r="L25" s="79"/>
       <c r="M25" s="79"/>
     </row>
-    <row r="26" spans="1:13" ht="13.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="112" t="s">
         <v>6</v>
       </c>
@@ -4130,7 +4105,9 @@
         <v>12</v>
       </c>
       <c r="I26" s="60"/>
-      <c r="J26" s="106"/>
+      <c r="J26" s="106" t="s">
+        <v>148</v>
+      </c>
       <c r="K26" s="41" t="s">
         <v>107</v>
       </c>
@@ -4169,7 +4146,7 @@
         <v>43482</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="111" t="s">
         <v>121</v>
       </c>
@@ -4294,7 +4271,7 @@
         <v>43469</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="112" t="s">
         <v>6</v>
       </c>
@@ -4417,7 +4394,7 @@
         <v>43490</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
         <v>6</v>
       </c>
@@ -4650,7 +4627,7 @@
       <c r="L43" s="79"/>
       <c r="M43" s="79"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="113" t="s">
         <v>6</v>
       </c>
@@ -4697,7 +4674,7 @@
       </c>
       <c r="P44" s="75"/>
     </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="112" t="s">
         <v>6</v>
       </c>
@@ -4725,7 +4702,7 @@
         <v>43482</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="112" t="s">
         <v>6</v>
       </c>
@@ -4759,7 +4736,7 @@
         <v>43459</v>
       </c>
     </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="112" t="s">
         <v>6</v>
       </c>
@@ -4787,7 +4764,7 @@
         <v>43462</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="112" t="s">
         <v>6</v>
       </c>
@@ -4815,7 +4792,7 @@
         <v>43469</v>
       </c>
     </row>
-    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="112" t="s">
         <v>6</v>
       </c>
@@ -4839,7 +4816,7 @@
       <c r="L49" s="79"/>
       <c r="M49" s="79"/>
     </row>
-    <row r="50" spans="1:16" ht="14.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="111" t="s">
         <v>121</v>
       </c>
@@ -4874,7 +4851,7 @@
         <v>43469</v>
       </c>
     </row>
-    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="112" t="s">
         <v>6</v>
       </c>
@@ -4925,7 +4902,7 @@
       </c>
       <c r="I52" s="121"/>
       <c r="J52" s="107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K52" s="41" t="s">
         <v>109</v>
@@ -4938,7 +4915,7 @@
       </c>
       <c r="P52" s="41"/>
     </row>
-    <row r="53" spans="1:16" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="123" t="s">
         <v>6</v>
       </c>
@@ -5153,7 +5130,7 @@
       <c r="L60" s="77"/>
       <c r="M60" s="77"/>
     </row>
-    <row r="61" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="113" t="s">
         <v>6</v>
       </c>
@@ -5183,7 +5160,7 @@
       <c r="L61" s="79"/>
       <c r="M61" s="79"/>
     </row>
-    <row r="62" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="113" t="s">
         <v>6</v>
       </c>
@@ -5207,7 +5184,7 @@
       <c r="L62" s="79"/>
       <c r="M62" s="79"/>
     </row>
-    <row r="63" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="111" t="s">
         <v>121</v>
       </c>
@@ -5242,7 +5219,7 @@
       <c r="N63" s="41"/>
       <c r="P63" s="41"/>
     </row>
-    <row r="64" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="113" t="s">
         <v>6</v>
       </c>
@@ -5266,7 +5243,7 @@
       <c r="L64" s="79"/>
       <c r="M64" s="79"/>
     </row>
-    <row r="65" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="113" t="s">
         <v>6</v>
       </c>
@@ -5290,7 +5267,7 @@
       <c r="L65" s="79"/>
       <c r="M65" s="79"/>
     </row>
-    <row r="66" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="113" t="s">
         <v>6</v>
       </c>
@@ -5338,7 +5315,7 @@
       <c r="L67" s="79"/>
       <c r="M67" s="79"/>
     </row>
-    <row r="68" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="113" t="s">
         <v>6</v>
       </c>
@@ -5368,7 +5345,7 @@
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
     </row>
-    <row r="69" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="113" t="s">
         <v>6</v>
       </c>
@@ -5392,7 +5369,7 @@
       <c r="L69" s="79"/>
       <c r="M69" s="79"/>
     </row>
-    <row r="70" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="113" t="s">
         <v>6</v>
       </c>
@@ -5416,7 +5393,7 @@
       <c r="L70" s="79"/>
       <c r="M70" s="79"/>
     </row>
-    <row r="71" spans="1:16" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="111" t="s">
         <v>121</v>
       </c>
@@ -5557,7 +5534,7 @@
         <v>48</v>
       </c>
       <c r="B75" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C75" s="42" t="s">
         <v>50</v>
@@ -5565,10 +5542,10 @@
       <c r="D75" s="43"/>
       <c r="E75" s="43"/>
       <c r="F75" s="130" t="s">
+        <v>124</v>
+      </c>
+      <c r="G75" s="130" t="s">
         <v>125</v>
-      </c>
-      <c r="G75" s="130" t="s">
-        <v>126</v>
       </c>
       <c r="H75" s="43"/>
       <c r="I75" s="43"/>
@@ -5579,7 +5556,7 @@
         <v>48</v>
       </c>
       <c r="B76" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C76" s="42" t="s">
         <v>50</v>
@@ -5587,10 +5564,10 @@
       <c r="D76" s="43"/>
       <c r="E76" s="43"/>
       <c r="F76" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G76" s="130" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H76" s="43"/>
       <c r="I76" s="43"/>
@@ -5601,7 +5578,7 @@
         <v>48</v>
       </c>
       <c r="B77" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C77" s="42" t="s">
         <v>50</v>
@@ -5609,7 +5586,7 @@
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
       <c r="F77" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G77" s="130" t="s">
         <v>59</v>
@@ -5623,7 +5600,7 @@
         <v>48</v>
       </c>
       <c r="B78" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C78" s="42" t="s">
         <v>50</v>
@@ -5631,10 +5608,10 @@
       <c r="D78" s="43"/>
       <c r="E78" s="43"/>
       <c r="F78" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G78" s="130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H78" s="43"/>
       <c r="I78" s="43"/>
@@ -5647,7 +5624,7 @@
         <v>48</v>
       </c>
       <c r="B79" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C79" s="42" t="s">
         <v>50</v>
@@ -5655,10 +5632,10 @@
       <c r="D79" s="43"/>
       <c r="E79" s="43"/>
       <c r="F79" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G79" s="130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H79" s="43"/>
       <c r="I79" s="43"/>
@@ -5669,7 +5646,7 @@
         <v>48</v>
       </c>
       <c r="B80" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C80" s="42" t="s">
         <v>50</v>
@@ -5677,10 +5654,10 @@
       <c r="D80" s="43"/>
       <c r="E80" s="43"/>
       <c r="F80" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G80" s="130" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H80" s="43"/>
       <c r="I80" s="43"/>
@@ -5693,7 +5670,7 @@
         <v>48</v>
       </c>
       <c r="B81" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C81" s="42" t="s">
         <v>50</v>
@@ -5701,10 +5678,10 @@
       <c r="D81" s="43"/>
       <c r="E81" s="43"/>
       <c r="F81" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G81" s="130" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H81" s="43"/>
       <c r="I81" s="43"/>
@@ -5715,7 +5692,7 @@
         <v>48</v>
       </c>
       <c r="B82" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C82" s="42" t="s">
         <v>50</v>
@@ -5723,10 +5700,10 @@
       <c r="D82" s="43"/>
       <c r="E82" s="43"/>
       <c r="F82" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G82" s="130" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H82" s="43"/>
       <c r="I82" s="43"/>
@@ -5737,7 +5714,7 @@
         <v>48</v>
       </c>
       <c r="B83" s="129" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C83" s="42" t="s">
         <v>50</v>
@@ -5745,10 +5722,10 @@
       <c r="D83" s="43"/>
       <c r="E83" s="43"/>
       <c r="F83" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G83" s="130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H83" s="43"/>
       <c r="I83" s="43"/>
@@ -5759,7 +5736,7 @@
         <v>48</v>
       </c>
       <c r="B84" s="131" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C84" s="116" t="s">
         <v>50</v>
@@ -5767,10 +5744,10 @@
       <c r="D84" s="132"/>
       <c r="E84" s="132"/>
       <c r="F84" s="130" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G84" s="130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H84" s="43"/>
       <c r="I84" s="43"/>
@@ -5781,7 +5758,7 @@
         <v>48</v>
       </c>
       <c r="B85" s="130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C85" s="130" t="s">
         <v>87</v>
@@ -5789,10 +5766,10 @@
       <c r="D85" s="130"/>
       <c r="E85" s="130"/>
       <c r="F85" s="130" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G85" s="130" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H85" s="43"/>
       <c r="I85" s="43"/>
@@ -5803,7 +5780,7 @@
         <v>48</v>
       </c>
       <c r="B86" s="130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C86" s="130" t="s">
         <v>87</v>
@@ -5811,10 +5788,10 @@
       <c r="D86" s="130"/>
       <c r="E86" s="130"/>
       <c r="F86" s="130" t="s">
+        <v>135</v>
+      </c>
+      <c r="G86" s="130" t="s">
         <v>136</v>
-      </c>
-      <c r="G86" s="130" t="s">
-        <v>137</v>
       </c>
       <c r="H86" s="126" t="s">
         <v>12</v>
@@ -5836,7 +5813,7 @@
         <v>48</v>
       </c>
       <c r="B87" s="130" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C87" s="130" t="s">
         <v>87</v>
@@ -5844,10 +5821,10 @@
       <c r="D87" s="130"/>
       <c r="E87" s="130"/>
       <c r="F87" s="130" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G87" s="130" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H87" s="126"/>
       <c r="I87" s="43"/>
@@ -5858,7 +5835,7 @@
         <v>48</v>
       </c>
       <c r="B88" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C88" s="42" t="s">
         <v>50</v>
@@ -5866,10 +5843,10 @@
       <c r="D88" s="43"/>
       <c r="E88" s="43"/>
       <c r="F88" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G88" s="130" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H88" s="43"/>
       <c r="I88" s="43"/>
@@ -5880,7 +5857,7 @@
         <v>48</v>
       </c>
       <c r="B89" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C89" s="42" t="s">
         <v>50</v>
@@ -5888,7 +5865,7 @@
       <c r="D89" s="43"/>
       <c r="E89" s="43"/>
       <c r="F89" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G89" s="130" t="s">
         <v>57</v>
@@ -5902,7 +5879,7 @@
         <v>48</v>
       </c>
       <c r="B90" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C90" s="42" t="s">
         <v>50</v>
@@ -5910,10 +5887,10 @@
       <c r="D90" s="43"/>
       <c r="E90" s="43"/>
       <c r="F90" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G90" s="130" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H90" s="43"/>
       <c r="I90" s="43"/>
@@ -5924,7 +5901,7 @@
         <v>48</v>
       </c>
       <c r="B91" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C91" s="42" t="s">
         <v>50</v>
@@ -5932,21 +5909,21 @@
       <c r="D91" s="43"/>
       <c r="E91" s="43"/>
       <c r="F91" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G91" s="130" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H91" s="43"/>
       <c r="I91" s="43"/>
       <c r="J91" s="43"/>
     </row>
-    <row r="92" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="42" t="s">
         <v>48</v>
       </c>
       <c r="B92" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C92" s="42" t="s">
         <v>50</v>
@@ -5954,17 +5931,17 @@
       <c r="D92" s="43"/>
       <c r="E92" s="43"/>
       <c r="F92" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G92" s="130" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H92" s="126" t="s">
         <v>12</v>
       </c>
       <c r="I92" s="43"/>
       <c r="J92" s="107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K92" s="41" t="s">
         <v>108</v>
@@ -5981,7 +5958,7 @@
         <v>48</v>
       </c>
       <c r="B93" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C93" s="42" t="s">
         <v>50</v>
@@ -5989,10 +5966,10 @@
       <c r="D93" s="43"/>
       <c r="E93" s="43"/>
       <c r="F93" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G93" s="130" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H93" s="43"/>
       <c r="I93" s="43"/>
@@ -6003,7 +5980,7 @@
         <v>48</v>
       </c>
       <c r="B94" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C94" s="42" t="s">
         <v>50</v>
@@ -6011,21 +5988,21 @@
       <c r="D94" s="43"/>
       <c r="E94" s="43"/>
       <c r="F94" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G94" s="130" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H94" s="43"/>
       <c r="I94" s="43"/>
       <c r="J94" s="43"/>
     </row>
-    <row r="95" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" ht="14.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="42" t="s">
         <v>48</v>
       </c>
       <c r="B95" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C95" s="42" t="s">
         <v>50</v>
@@ -6033,17 +6010,17 @@
       <c r="D95" s="43"/>
       <c r="E95" s="43"/>
       <c r="F95" s="130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G95" s="130" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H95" s="36" t="s">
         <v>12</v>
       </c>
       <c r="I95" s="43"/>
       <c r="J95" s="107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K95" s="41" t="s">
         <v>108</v>
@@ -6064,7 +6041,7 @@
     </filterColumn>
     <filterColumn colId="10">
       <filters>
-        <filter val="ngocnv"/>
+        <filter val="khoand"/>
       </filters>
     </filterColumn>
     <sortState ref="A11:P71">

</xml_diff>